<commit_message>
Remove unused columns in BOM for kitspace compatibility
</commit_message>
<xml_diff>
--- a/pcb_design/Sangaboard v3 BOM.xlsx
+++ b/pcb_design/Sangaboard v3 BOM.xlsx
@@ -209,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,14 +244,6 @@
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -313,7 +305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,27 +326,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,23 +334,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,11 +350,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,22 +437,21 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.06"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.86"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="8" style="0" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="11" style="0" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="23" style="0" width="14.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="7" style="0" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="17" style="0" width="14.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -501,29 +464,29 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -536,35 +499,11 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E2" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F2" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"amphenol-icc-fci")</f>
-        <v>amphenol-icc-fci</v>
-      </c>
-      <c r="G2" s="2" t="str">
+      <c r="D2" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"87520-0010blf")</f>
         <v>87520-0010blf</v>
       </c>
-      <c r="H2" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"usb-2-0-type-a-plug-cable")</f>
-        <v>usb-2-0-type-a-plug-cable</v>
-      </c>
-      <c r="I2" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J2" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2112381?MER=sy-me-pd-mi-alte")</f>
-        <v>2112381?MER=sy-me-pd-mi-alte</v>
-      </c>
-      <c r="K2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>2112381</v>
       </c>
     </row>
@@ -578,35 +517,11 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F3" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"hirose-hrs")</f>
-        <v>hirose-hrs</v>
-      </c>
-      <c r="G3" s="2" t="str">
+      <c r="D3" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"zx62d-b-5p8-30")</f>
         <v>zx62d-b-5p8-30</v>
       </c>
-      <c r="H3" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"micro-usb-2-0-type-b-rcpt-smt")</f>
-        <v>micro-usb-2-0-type-b-rcpt-smt</v>
-      </c>
-      <c r="I3" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),2554980)</f>
-        <v>2554980</v>
-      </c>
-      <c r="K3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>2554980</v>
       </c>
     </row>
@@ -617,534 +532,312 @@
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E4" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F4" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kemet")</f>
-        <v>kemet</v>
-      </c>
-      <c r="G4" s="2" t="str">
+      <c r="D4" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"c0805y104k4racauto")</f>
         <v>c0805y104k4racauto</v>
       </c>
-      <c r="H4" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cap-0-1-f-16v-10-x7r-0805")</f>
-        <v>cap-0-1-f-16v-10-x7r-0805</v>
-      </c>
-      <c r="I4" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J4" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2673142?st=100nf%2016V%200805")</f>
-        <v>2673142?st=100nf%2016V%200805</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>2673142</v>
       </c>
     </row>
-    <row r="5" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+    <row r="5" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E5" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F5" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"wurth-elektronik")</f>
-        <v>wurth-elektronik</v>
-      </c>
-      <c r="G5" s="12" t="n">
+      <c r="D5" s="8" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),885012007030)</f>
         <v>885012007030</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cap-mlcc-np0-22pf-25v-0805")</f>
-        <v>cap-mlcc-np0-22pf-25v-0805</v>
-      </c>
-      <c r="I5" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J5" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2533861?st=22pF%20capacitor")</f>
-        <v>2533861?st=22pF%20capacitor</v>
-      </c>
-      <c r="K5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>2533861</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+    <row r="6" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E6" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F6" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"panasonic-electronic-components")</f>
-        <v>panasonic-electronic-components</v>
-      </c>
-      <c r="G6" s="15" t="str">
+      <c r="D6" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"eee1ca100sr")</f>
         <v>eee1ca100sr</v>
       </c>
-      <c r="H6" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cap-alu-elec-10uf-16v-smd")</f>
-        <v>cap-alu-elec-10uf-16v-smd</v>
-      </c>
-      <c r="I6" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J6" s="10" t="n">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),9696920)</f>
+      <c r="E6" s="9" t="n">
         <v>9696920</v>
       </c>
-      <c r="K6" s="10" t="n">
-        <v>9696920</v>
-      </c>
+      <c r="AMD6" s="0"/>
+      <c r="AME6" s="0"/>
+      <c r="AMF6" s="0"/>
+      <c r="AMG6" s="0"/>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+    <row r="7" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="13" t="n">
+      <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E7" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F7" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"avx")</f>
-        <v>avx</v>
-      </c>
-      <c r="G7" s="15" t="str">
+      <c r="D7" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"08053c105jat2a")</f>
         <v>08053c105jat2a</v>
       </c>
-      <c r="H7" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cap-mlcc-x7r-1uf-25v-0805")</f>
-        <v>cap-mlcc-x7r-1uf-25v-0805</v>
-      </c>
-      <c r="I7" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J7" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2332736?st=SMD%20Multilayer%20Ceramic%20Capacitor,%200805%20[2012%20Metric],%201%20µF,%2025%20V,")</f>
-        <v>2332736?st=SMD%20Multilayer%20Ceramic%20Capacitor,%200805%20[2012%20Metric],%201%20µF,%2025%20V,</v>
-      </c>
-      <c r="K7" s="10" t="n">
+      <c r="E7" s="9" t="n">
         <v>2332736</v>
       </c>
+      <c r="AMD7" s="0"/>
+      <c r="AME7" s="0"/>
+      <c r="AMF7" s="0"/>
+      <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+    <row r="8" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13" t="n">
+      <c r="B8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E8" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F8" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"panasonic-electronic-components")</f>
-        <v>panasonic-electronic-components</v>
-      </c>
-      <c r="G8" s="15" t="str">
+      <c r="D8" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"db2w31900l")</f>
         <v>db2w31900l</v>
       </c>
-      <c r="H8" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"diode-schottky-30v-mini2-f3-b")</f>
-        <v>diode-schottky-30v-mini2-f3-b</v>
-      </c>
-      <c r="I8" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J8" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2284956?st=Schottky%20Rectifier,%2040%20V,%203%20A,%20Single,%20SOD-123F,%202%20Pins")</f>
-        <v>2284956?st=Schottky%20Rectifier,%2040%20V,%203%20A,%20Single,%20SOD-123F,%202%20Pins</v>
-      </c>
-      <c r="K8" s="10" t="n">
+      <c r="E8" s="9" t="n">
         <v>2284956</v>
       </c>
+      <c r="AMD8" s="0"/>
+      <c r="AME8" s="0"/>
+      <c r="AMF8" s="0"/>
+      <c r="AMG8" s="0"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="13" t="n">
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E9" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F9" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"bourns")</f>
-        <v>bourns</v>
-      </c>
-      <c r="G9" s="15" t="str">
+      <c r="D9" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cd1206-s01575")</f>
         <v>cd1206-s01575</v>
       </c>
-      <c r="H9" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"diode-switching-100v-150ma-1206")</f>
-        <v>diode-switching-100v-150ma-1206</v>
-      </c>
-      <c r="I9" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J9" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2211947?st=CD1206-S01575")</f>
-        <v>2211947?st=CD1206-S01575</v>
-      </c>
-      <c r="K9" s="10" t="n">
+      <c r="E9" s="9" t="n">
         <v>2211947</v>
       </c>
+      <c r="AMD9" s="0"/>
+      <c r="AME9" s="0"/>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+    <row r="10" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13" t="n">
+      <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E10" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F10" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kingbright")</f>
-        <v>kingbright</v>
-      </c>
-      <c r="G10" s="15" t="str">
+      <c r="D10" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kp-1608ec")</f>
         <v>kp-1608ec</v>
       </c>
-      <c r="H10" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"led-red-8mcd-625nm-smd")</f>
-        <v>led-red-8mcd-625nm-smd</v>
-      </c>
-      <c r="I10" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J10" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2463988?st=LOW%20POWER%20LED")</f>
-        <v>2463988?st=LOW%20POWER%20LED</v>
-      </c>
-      <c r="K10" s="10" t="n">
+      <c r="E10" s="9" t="n">
         <v>2463988</v>
       </c>
+      <c r="AMD10" s="0"/>
+      <c r="AME10" s="0"/>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+    <row r="11" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="13" t="n">
+      <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E11" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F11" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kingbright")</f>
-        <v>kingbright</v>
-      </c>
-      <c r="G11" s="15" t="str">
+      <c r="D11" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kp-1608cgck")</f>
         <v>kp-1608cgck</v>
       </c>
-      <c r="H11" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"led-0603-50mcd-green")</f>
-        <v>led-0603-50mcd-green</v>
-      </c>
-      <c r="I11" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J11" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2290328?st=LOW%20POWER%20LED")</f>
-        <v>2290328?st=LOW%20POWER%20LED</v>
-      </c>
-      <c r="K11" s="10" t="n">
+      <c r="E11" s="9" t="n">
         <v>2290328</v>
       </c>
+      <c r="AMD11" s="0"/>
+      <c r="AME11" s="0"/>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+    <row r="12" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="13" t="n">
+      <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E12" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F12" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kingbright")</f>
-        <v>kingbright</v>
-      </c>
-      <c r="G12" s="15" t="str">
+      <c r="D12" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kpt-1608yc")</f>
         <v>kpt-1608yc</v>
       </c>
-      <c r="H12" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"led-0603-yellow-8mcd-588nm")</f>
-        <v>led-0603-yellow-8mcd-588nm</v>
-      </c>
-      <c r="I12" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J12" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2099227?ost=2099227&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>2099227?ost=2099227&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K12" s="10" t="n">
+      <c r="E12" s="9" t="n">
         <v>2099227</v>
       </c>
+      <c r="AMD12" s="0"/>
+      <c r="AME12" s="0"/>
+      <c r="AMF12" s="0"/>
+      <c r="AMG12" s="0"/>
+      <c r="AMH12" s="0"/>
+      <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="13" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="13" t="n">
+      <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E13" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F13" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kingbright")</f>
-        <v>kingbright</v>
-      </c>
-      <c r="G13" s="15" t="str">
+      <c r="D13" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kp-1608qbc-d")</f>
         <v>kp-1608qbc-d</v>
       </c>
-      <c r="H13" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"led-smd-0603-blue")</f>
-        <v>led-smd-0603-blue</v>
-      </c>
-      <c r="I13" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J13" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2217972?st=KPT-1608YC%20-%20%20LED,%20Low%20Power,%20Blue")</f>
-        <v>2217972?st=KPT-1608YC%20-%20%20LED,%20Low%20Power,%20Blue</v>
-      </c>
-      <c r="K13" s="10" t="n">
+      <c r="E13" s="9" t="n">
         <v>2217972</v>
       </c>
+      <c r="AMD13" s="0"/>
+      <c r="AME13" s="0"/>
+      <c r="AMF13" s="0"/>
+      <c r="AMG13" s="0"/>
+      <c r="AMH13" s="0"/>
+      <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
+    <row r="14" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="13" t="n">
+      <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E14" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F14" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"bourns")</f>
-        <v>bourns</v>
-      </c>
-      <c r="G14" s="15" t="str">
+      <c r="D14" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cd-hd2004")</f>
         <v>cd-hd2004</v>
       </c>
-      <c r="H14" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"diode-bridge-rect-1-ph-40v-smd")</f>
-        <v>diode-bridge-rect-1-ph-40v-smd</v>
-      </c>
-      <c r="I14" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J14" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2676044?krypto=HaflPpNLuHOFLHN6OxuHJMFd%2BijEvhI0duXna044V4ieLdAyHfbvP5zEqBpvqb3tSU5DiOtHH9J8%2Bn4HqqDhFw%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>2676044?krypto=HaflPpNLuHOFLHN6OxuHJMFd%2BijEvhI0duXna044V4ieLdAyHfbvP5zEqBpvqb3tSU5DiOtHH9J8%2Bn4HqqDhFw%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K14" s="10" t="n">
+      <c r="E14" s="9" t="n">
         <v>2676044</v>
       </c>
+      <c r="AMD14" s="0"/>
+      <c r="AME14" s="0"/>
+      <c r="AMF14" s="0"/>
+      <c r="AMG14" s="0"/>
+      <c r="AMH14" s="0"/>
+      <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+    <row r="15" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E15" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F15" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"littelfuse")</f>
-        <v>littelfuse</v>
-      </c>
-      <c r="G15" s="12" t="str">
+      <c r="D15" s="8" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"minismdc260f-2")</f>
         <v>minismdc260f-2</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"polyswitch-smd-1812-2-6a")</f>
-        <v>polyswitch-smd-1812-2-6a</v>
-      </c>
-      <c r="I15" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J15" s="7" t="n">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),1345935)</f>
+      <c r="E15" s="6" t="n">
         <v>1345935</v>
       </c>
-      <c r="K15" s="7" t="n">
-        <v>1345935</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="AMD15" s="0"/>
+      <c r="AME15" s="0"/>
+      <c r="AMF15" s="0"/>
+      <c r="AMG15" s="0"/>
+      <c r="AMH15" s="0"/>
+      <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1157,35 +850,11 @@
       <c r="C16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E16" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F16" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"littelfuse")</f>
-        <v>littelfuse</v>
-      </c>
-      <c r="G16" s="2" t="str">
+      <c r="D16" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1210l035yr")</f>
         <v>1210l035yr</v>
       </c>
-      <c r="H16" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"polyfuse-ptc-1210-0-35a")</f>
-        <v>polyfuse-ptc-1210-0-35a</v>
-      </c>
-      <c r="I16" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),1822207)</f>
-        <v>1822207</v>
-      </c>
-      <c r="K16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>1822207</v>
       </c>
     </row>
@@ -1199,35 +868,11 @@
       <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E17" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F17" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"littelfuse")</f>
-        <v>littelfuse</v>
-      </c>
-      <c r="G17" s="2" t="str">
+      <c r="D17" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1206l050yr")</f>
         <v>1206l050yr</v>
       </c>
-      <c r="H17" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"fuse-resettable-1206-6v-500ma")</f>
-        <v>fuse-resettable-1206-6v-500ma</v>
-      </c>
-      <c r="I17" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J17" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1596993?ost=1596993&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>1596993?ost=1596993&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K17" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>1596993</v>
       </c>
     </row>
@@ -1241,40 +886,16 @@
       <c r="C18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E18" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F18" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"tdk")</f>
-        <v>tdk</v>
-      </c>
-      <c r="G18" s="2" t="str">
+      <c r="D18" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"mpz2012s601a")</f>
         <v>mpz2012s601a</v>
       </c>
-      <c r="H18" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"ferrite-bead-0-1ohm-2a-0805")</f>
-        <v>ferrite-bead-0-1ohm-2a-0805</v>
-      </c>
-      <c r="I18" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J18" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1669753?krypto=pMnlyQddMKTtnSihmqgvLosEEzd2cAKvNg7xDsx5mDFep%2BmTNOTdaG4z%2BrM3Rjigbmp6qVL%2FD0NwlcmmAVGi2A%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>1669753?krypto=pMnlyQddMKTtnSihmqgvLosEEzd2cAKvNg7xDsx5mDFep%2BmTNOTdaG4z%2BrM3Rjigbmp6qVL%2FD0NwlcmmAVGi2A%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K18" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>1669753</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="1" t="n">
@@ -1283,35 +904,11 @@
       <c r="C19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E19" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F19" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"wurth-elektronik")</f>
-        <v>wurth-elektronik</v>
-      </c>
-      <c r="G19" s="2" t="n">
+      <c r="D19" s="2" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),742792031)</f>
         <v>742792031</v>
       </c>
-      <c r="H19" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"ferrite-bead-0-05ohm-3a-0805")</f>
-        <v>ferrite-bead-0-05ohm-3a-0805</v>
-      </c>
-      <c r="I19" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J19" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1635734?st=Ferrite%20Bead,%200805%20[2012%20Metric],%20600%20ohm,%203%20A,")</f>
-        <v>1635734?st=Ferrite%20Bead,%200805%20[2012%20Metric],%20600%20ohm,%203%20A,</v>
-      </c>
-      <c r="K19" s="0" t="n">
+      <c r="E19" s="0" t="n">
         <v>1635734</v>
       </c>
     </row>
@@ -1325,35 +922,11 @@
       <c r="C20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E20" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F20" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"jst-japan-solderless-terminals")</f>
-        <v>jst-japan-solderless-terminals</v>
-      </c>
-      <c r="G20" s="2" t="str">
+      <c r="D20" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"s5b-xh-a-lf-sn")</f>
         <v>s5b-xh-a-lf-sn</v>
       </c>
-      <c r="H20" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"header-right-angle-5way")</f>
-        <v>header-right-angle-5way</v>
-      </c>
-      <c r="I20" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J20" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1516293?ost=1516293&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>1516293?ost=1516293&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K20" s="0" t="n">
+      <c r="E20" s="0" t="n">
         <v>1516293</v>
       </c>
     </row>
@@ -1367,35 +940,11 @@
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E21" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F21" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"panasonic-electronic-components")</f>
-        <v>panasonic-electronic-components</v>
-      </c>
-      <c r="G21" s="2" t="str">
+      <c r="D21" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"erj6geyj103v")</f>
         <v>erj6geyj103v</v>
       </c>
-      <c r="H21" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"res-thick-film-10k-5-0-125w-0805")</f>
-        <v>res-thick-film-10k-5-0-125w-0805</v>
-      </c>
-      <c r="I21" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J21" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2057719?MER=sy-me-pd-mi-alte&amp;st=10k%20SMD%20RESISTOR")</f>
-        <v>2057719?MER=sy-me-pd-mi-alte&amp;st=10k%20SMD%20RESISTOR</v>
-      </c>
-      <c r="K21" s="0" t="n">
+      <c r="E21" s="0" t="n">
         <v>2057719</v>
       </c>
     </row>
@@ -1409,35 +958,11 @@
       <c r="C22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E22" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F22" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"panasonic-electronic-components")</f>
-        <v>panasonic-electronic-components</v>
-      </c>
-      <c r="G22" s="2" t="str">
+      <c r="D22" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"erj6geyj220v")</f>
         <v>erj6geyj220v</v>
       </c>
-      <c r="H22" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"res-thick-film-22r-5-0-125w-0805")</f>
-        <v>res-thick-film-22r-5-0-125w-0805</v>
-      </c>
-      <c r="I22" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J22" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2057672?st=SMD%20Chip%20Resistor,%2022%20ohm,%20150%20V,%20Thick%20Film,%200805%20[2012%20Metric],%20125%20mW")</f>
-        <v>2057672?st=SMD%20Chip%20Resistor,%2022%20ohm,%20150%20V,%20Thick%20Film,%200805%20[2012%20Metric],%20125%20mW</v>
-      </c>
-      <c r="K22" s="0" t="n">
+      <c r="E22" s="0" t="n">
         <v>2057672</v>
       </c>
     </row>
@@ -1451,35 +976,11 @@
       <c r="C23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E23" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F23" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"panasonic-electronic-components")</f>
-        <v>panasonic-electronic-components</v>
-      </c>
-      <c r="G23" s="2" t="str">
+      <c r="D23" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"exb38v102jv")</f>
         <v>exb38v102jv</v>
       </c>
-      <c r="H23" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"resistor-cvex-array-0603x4-1k")</f>
-        <v>resistor-cvex-array-0603x4-1k</v>
-      </c>
-      <c r="I23" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J23" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2060100?ost=2060100&amp;scope=partnumberlookahead&amp;exaMfpn=true&amp;searchref=searchlookahead&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fw%2Fsearch")</f>
-        <v>2060100?ost=2060100&amp;scope=partnumberlookahead&amp;exaMfpn=true&amp;searchref=searchlookahead&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fw%2Fsearch</v>
-      </c>
-      <c r="K23" s="0" t="n">
+      <c r="E23" s="0" t="n">
         <v>2060100</v>
       </c>
     </row>
@@ -1493,35 +994,11 @@
       <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E24" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F24" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"bourns")</f>
-        <v>bourns</v>
-      </c>
-      <c r="G24" s="2" t="str">
+      <c r="D24" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cg0603mlc-05e")</f>
         <v>cg0603mlc-05e</v>
       </c>
-      <c r="H24" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"varistor-supp-esd-protect-20v")</f>
-        <v>varistor-supp-esd-protect-20v</v>
-      </c>
-      <c r="I24" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J24" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1838966?ost=1838966&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>1838966?ost=1838966&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K24" s="0" t="n">
+      <c r="E24" s="0" t="n">
         <v>1838966</v>
       </c>
     </row>
@@ -1535,35 +1012,11 @@
       <c r="C25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E25" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F25" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"microchip")</f>
-        <v>microchip</v>
-      </c>
-      <c r="G25" s="2" t="str">
+      <c r="D25" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"atmega32u4-au")</f>
         <v>atmega32u4-au</v>
       </c>
-      <c r="H25" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"mcu-8bit-megaavr-16mhz-tqfp-44")</f>
-        <v>mcu-8bit-megaavr-16mhz-tqfp-44</v>
-      </c>
-      <c r="I25" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J25" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1748525?st=ATMEGA32U4")</f>
-        <v>1748525?st=ATMEGA32U4</v>
-      </c>
-      <c r="K25" s="0" t="n">
+      <c r="E25" s="0" t="n">
         <v>1748525</v>
       </c>
     </row>
@@ -1577,35 +1030,11 @@
       <c r="C26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E26" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F26" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"on-semiconductor")</f>
-        <v>on-semiconductor</v>
-      </c>
-      <c r="G26" s="2" t="str">
+      <c r="D26" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uln2003adr2g")</f>
         <v>uln2003adr2g</v>
       </c>
-      <c r="H26" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"trans-npn-50v-0-5a-soic-16")</f>
-        <v>trans-npn-50v-0-5a-soic-16</v>
-      </c>
-      <c r="I26" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J26" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2628016?st=ULN2003")</f>
-        <v>2628016?st=ULN2003</v>
-      </c>
-      <c r="K26" s="0" t="n">
+      <c r="E26" s="0" t="n">
         <v>2628016</v>
       </c>
     </row>
@@ -1619,98 +1048,57 @@
       <c r="C27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E27" s="5" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F27" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"abracon")</f>
-        <v>abracon</v>
-      </c>
-      <c r="G27" s="2" t="str">
+      <c r="D27" s="2" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"abm8-16-000mhz-b2-t")</f>
         <v>abm8-16-000mhz-b2-t</v>
       </c>
-      <c r="H27" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"crystal-16mhz-18pf-cl-3-2x2-5mm")</f>
-        <v>crystal-16mhz-18pf-cl-3-2x2-5mm</v>
-      </c>
-      <c r="I27" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J27" s="0" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1611819?ost=1611819&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch")</f>
-        <v>1611819?ost=1611819&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</v>
-      </c>
-      <c r="K27" s="0" t="n">
+      <c r="E27" s="0" t="n">
         <v>1611819</v>
       </c>
     </row>
-    <row r="28" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+    <row r="28" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="8" t="n">
+      <c r="B28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="10" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("split(D2,""/"")"),"http:")</f>
-        <v>http:</v>
-      </c>
-      <c r="E28" s="11" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uk.farnell.com")</f>
-        <v>uk.farnell.com</v>
-      </c>
-      <c r="F28" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"multicomp")</f>
-        <v>multicomp</v>
-      </c>
-      <c r="G28" s="12" t="str">
+      <c r="D28" s="8" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2213s-50g")</f>
         <v>2213s-50g</v>
       </c>
-      <c r="H28" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"connector-header-50pos-2-54mm")</f>
-        <v>connector-header-50pos-2-54mm</v>
-      </c>
-      <c r="I28" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"dp")</f>
-        <v>dp</v>
-      </c>
-      <c r="J28" s="7" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2847228?st=2%20row%20header%20male")</f>
-        <v>2847228?st=2%20row%20header%20male</v>
-      </c>
-      <c r="K28" s="7" t="n">
+      <c r="E28" s="6" t="n">
         <v>2847228</v>
       </c>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="AMD28" s="0"/>
+      <c r="AME28" s="0"/>
+      <c r="AMF28" s="0"/>
+      <c r="AMG28" s="0"/>
+      <c r="AMH28" s="0"/>
+      <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18" t="s">
+      <c r="B30" s="0"/>
+      <c r="F30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="19" t="n">
+      <c r="G30" s="12" t="n">
         <f aca="false">SUM(B2:B28)</f>
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Find parts for Digikey/Mouser/RS
</commit_message>
<xml_diff>
--- a/pcb_design/Sangaboard v3 BOM.xlsx
+++ b/pcb_design/Sangaboard v3 BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -28,10 +28,19 @@
     <t xml:space="preserve">QTY</t>
   </si>
   <si>
-    <t xml:space="preserve">Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Part number (from link)</t>
+    <t xml:space="preserve">Manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
   </si>
   <si>
     <t xml:space="preserve">Farnell</t>
@@ -40,163 +49,322 @@
     <t xml:space="preserve">USB Type A</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/amphenol-icc-fci/87520-0010blf/usb-2-0-type-a-plug-cable/dp/2112381?MER=sy-me-pd-mi-alte</t>
+    <t xml:space="preserve">FCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87520-0010BLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">609-1045-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">649875200010BLF</t>
   </si>
   <si>
     <t xml:space="preserve">USB Type B Micro</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/hirose-hrs/zx62d-b-5p8-30/micro-usb-2-0-type-b-rcpt-smt/dp/2554980</t>
+    <t xml:space="preserve">Hirose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZX62D-B-5P8(30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H125272CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">798ZX62DB5P830</t>
   </si>
   <si>
     <t xml:space="preserve">C1, C5, C9</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/kemet/c0805y104k4racauto/cap-0-1-f-16v-10-x7r-0805/dp/2673142?st=100nf%2016V%200805</t>
+    <t xml:space="preserve">KEMET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0805Y104K4RACAUTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80C0805Y104K4RAUTO</t>
   </si>
   <si>
     <t xml:space="preserve">C2, C3</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/wurth-elektronik/885012007030/cap-mlcc-np0-22pf-25v-0805/dp/2533861?st=22pF%20capacitor</t>
+    <t xml:space="preserve">Würth Elektronik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732-7829-6-ND</t>
   </si>
   <si>
     <t xml:space="preserve">C4, C8</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/panasonic-electronic-components/eee1ca100sr/cap-alu-elec-10uf-16v-smd/dp/9696920</t>
+    <t xml:space="preserve">Panasonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEE-1CA100SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCE3878CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667EEE1CA100SR</t>
   </si>
   <si>
     <t xml:space="preserve">C6, C7, C10, C11</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/avx/08053c105jat2a/cap-mlcc-x7r-1uf-25v-0805/dp/2332736?st=SMD%20Multilayer%20Ceramic%20Capacitor,%200805%20[2012%20Metric],%201%20µF,%2025%20V,</t>
+    <t xml:space="preserve">AVX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08053C105JAT2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">478-10487-6-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58108053C105JAT2A</t>
   </si>
   <si>
     <t xml:space="preserve">D1, D2, D3, D4</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/panasonic-electronic-components/db2w31900l/diode-schottky-30v-mini2-f3-b/dp/2284956?st=Schottky%20Rectifier,%2040%20V,%203%20A,%20Single,%20SOD-123F,%202%20Pins</t>
+    <t xml:space="preserve">DB2W31900L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2W31900LCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">D5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/bourns/cd1206-s01575/diode-switching-100v-150ma-1206/dp/2211947?st=CD1206-S01575</t>
+    <t xml:space="preserve">Bourns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD1206-S01575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD1206-S01575TR-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652CD1206S01575</t>
   </si>
   <si>
     <t xml:space="preserve">D6</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/kingbright/kp-1608ec/led-red-8mcd-625nm-smd/dp/2463988?st=LOW%20POWER%20LED</t>
+    <t xml:space="preserve">Kingbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP-1608EC</t>
   </si>
   <si>
     <t xml:space="preserve">D7</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/kingbright/kp-1608cgck/led-0603-50mcd-green/dp/2290328?st=LOW%20POWER%20LED</t>
+    <t xml:space="preserve">KP-1608CGCK</t>
   </si>
   <si>
     <t xml:space="preserve">D8</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/kingbright/kpt-1608yc/led-0603-yellow-8mcd-588nm/dp/2099227?ost=2099227&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">KPT-1608YC</t>
   </si>
   <si>
     <t xml:space="preserve">D9</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/kingbright/kp-1608qbc-d/led-smd-0603-blue/dp/2217972?st=KPT-1608YC%20-%20%20LED,%20Low%20Power,%20Blue</t>
+    <t xml:space="preserve">KP-1608QBC-D</t>
   </si>
   <si>
     <t xml:space="preserve">D10</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/bourns/cd-hd2004/diode-bridge-rect-1-ph-40v-smd/dp/2676044?krypto=HaflPpNLuHOFLHN6OxuHJMFd%2BijEvhI0duXna044V4ieLdAyHfbvP5zEqBpvqb3tSU5DiOtHH9J8%2Bn4HqqDhFw%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">CD-HD2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD-HD2004CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652CDHD2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1261771P</t>
   </si>
   <si>
     <t xml:space="preserve">F1</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/littelfuse/minismdc260f-2/polyswitch-smd-1812-2-6a/dp/1345935</t>
+    <t xml:space="preserve">Littelfuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINISMDC260F-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINISMDC260F-2CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">650MINISMDC260F2</t>
   </si>
   <si>
     <t xml:space="preserve">F2, F3, F4</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/littelfuse/1210l035yr/polyfuse-ptc-1210-0-35a/dp/1822207</t>
+    <t xml:space="preserve">1210L035YR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2997CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5761210L035</t>
   </si>
   <si>
     <t xml:space="preserve">F5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/littelfuse/1206l050yr/fuse-resettable-1206-6v-500ma/dp/1596993?ost=1596993&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">1206L050YR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2112CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5761206L050YR</t>
   </si>
   <si>
     <t xml:space="preserve">L1</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/tdk/mpz2012s601a/ferrite-bead-0-1ohm-2a-0805/dp/1669753?krypto=pMnlyQddMKTtnSihmqgvLosEEzd2cAKvNg7xDsx5mDFep%2BmTNOTdaG4z%2BrM3Rjigbmp6qVL%2FD0NwlcmmAVGi2A%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">TDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPZ2012S601A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">810MPZ2012S601A</t>
   </si>
   <si>
     <t xml:space="preserve">L2</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/wurth-elektronik/742792031/ferrite-bead-0-05ohm-3a-0805/dp/1635734?st=Ferrite%20Bead,%200805%20[2012%20Metric],%20600%20ohm,%203%20A,</t>
+    <t xml:space="preserve">732-4638-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">J12, J13, J14</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/jst-japan-solderless-terminals/s5b-xh-a-lf-sn/header-right-angle-5way/dp/1516293?ost=1516293&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">JST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S5B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">455-2242-ND</t>
   </si>
   <si>
     <t xml:space="preserve">R1, R2, R5, R6</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/panasonic-electronic-components/erj6geyj103v/res-thick-film-10k-5-0-125w-0805/dp/2057719?MER=sy-me-pd-mi-alte&amp;st=10k%20SMD%20RESISTOR</t>
+    <t xml:space="preserve">ERJ-6GEYJ103V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10KACT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667ERJ6GEYJ103V</t>
   </si>
   <si>
     <t xml:space="preserve">R3, R4</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/panasonic-electronic-components/erj6geyj220v/res-thick-film-22r-5-0-125w-0805/dp/2057672?st=SMD%20Chip%20Resistor,%2022%20ohm,%20150%20V,%20Thick%20Film,%200805%20[2012%20Metric],%20125%20mW</t>
+    <t xml:space="preserve">ERJ-6GEYJ220V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P22ACT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667ERJ6GEYJ220V</t>
   </si>
   <si>
     <t xml:space="preserve">RN1</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/panasonic-electronic-components/exb38v102jv/resistor-cvex-array-0603x4-1k/dp/2060100?ost=2060100&amp;scope=partnumberlookahead&amp;exaMfpn=true&amp;searchref=searchlookahead&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fw%2Fsearch</t>
+    <t xml:space="preserve">EXB-38V102JV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y9102CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667EXB38V102JV</t>
   </si>
   <si>
     <t xml:space="preserve">RV1, VR2</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/bourns/cg0603mlc-05e/varistor-supp-esd-protect-20v/dp/1838966?ost=1838966&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">CG0603MLC-05E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG0603MLC-05ECT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652CG0603MLC05E</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/microchip/atmega32u4-au/mcu-8bit-megaavr-16mhz-tqfp-44/dp/1748525?st=ATMEGA32U4</t>
+    <t xml:space="preserve">Microchip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATMEGA32U4-AU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATMEGA32U4-AU-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">556ATMEGA32U4AU</t>
   </si>
   <si>
     <t xml:space="preserve">U2, U3</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/on-semiconductor/uln2003adr2g/trans-npn-50v-0-5a-soic-16/dp/2628016?st=ULN2003</t>
+    <t xml:space="preserve">ON Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULN2003ADR2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULN2003ADR2GOSCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863ULN2003ADR2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1868994P</t>
   </si>
   <si>
     <t xml:space="preserve">Y1</t>
   </si>
   <si>
-    <t xml:space="preserve">http://uk.farnell.com/abracon/abm8-16-000mhz-b2-t/crystal-16mhz-18pf-cl-3-2x2-5mm/dp/1611819?ost=1611819&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch</t>
+    <t xml:space="preserve">Abracon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABM8-16.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">535-9134-6-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">815ABM816B2T</t>
   </si>
   <si>
     <t xml:space="preserve">Male headers</t>
   </si>
   <si>
-    <t xml:space="preserve">https://uk.farnell.com/multicomp/2213s-50g/connector-header-50pos-2-54mm/dp/2847228?st=2%20row%20header%20male</t>
+    <t xml:space="preserve">Multicomp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2213S-50G</t>
   </si>
   <si>
     <t xml:space="preserve">Total parts:</t>
@@ -209,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -236,14 +404,6 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -305,7 +465,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,24 +482,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -350,11 +502,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,66 +519,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -438,13 +530,13 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.73"/>
@@ -461,18 +553,24 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -491,86 +589,109 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"87520-0010blf")</f>
-        <v>87520-0010blf</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>7710057</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>2112381</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"zx62d-b-5p8-30")</f>
-        <v>zx62d-b-5p8-30</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1361405</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>2554980</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"c0805y104k4racauto")</f>
-        <v>c0805y104k4racauto</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>2673142</v>
       </c>
     </row>
-    <row r="5" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7" t="n">
+    <row r="5" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),885012007030)</f>
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>885012007030</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>710885012007030</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1814032</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>2533861</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
       <c r="AMD5" s="0"/>
       <c r="AME5" s="0"/>
       <c r="AMF5" s="0"/>
@@ -579,21 +700,29 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
+    <row r="6" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"eee1ca100sr")</f>
-        <v>eee1ca100sr</v>
-      </c>
-      <c r="E6" s="9" t="n">
+      <c r="C6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>9206828</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>9696920</v>
       </c>
       <c r="AMD6" s="0"/>
@@ -604,21 +733,27 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>15</v>
+    <row r="7" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"08053c105jat2a")</f>
-        <v>08053c105jat2a</v>
-      </c>
-      <c r="E7" s="9" t="n">
+      <c r="C7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0" t="n">
         <v>2332736</v>
       </c>
       <c r="AMD7" s="0"/>
@@ -629,21 +764,27 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>17</v>
+    <row r="8" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"db2w31900l")</f>
-        <v>db2w31900l</v>
-      </c>
-      <c r="E8" s="9" t="n">
+      <c r="C8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0" t="n">
+        <v>7240321</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>2284956</v>
       </c>
       <c r="AMD8" s="0"/>
@@ -654,21 +795,29 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
+    <row r="9" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cd1206-s01575")</f>
-        <v>cd1206-s01575</v>
-      </c>
-      <c r="E9" s="9" t="n">
+      <c r="C9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>7734514</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>2211947</v>
       </c>
       <c r="AMD9" s="0"/>
@@ -679,21 +828,25 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>21</v>
+    <row r="10" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kp-1608ec")</f>
-        <v>kp-1608ec</v>
-      </c>
-      <c r="E10" s="9" t="n">
+      <c r="C10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0" t="n">
+        <v>8610018</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>2463988</v>
       </c>
       <c r="AMD10" s="0"/>
@@ -704,21 +857,25 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>23</v>
+    <row r="11" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kp-1608cgck")</f>
-        <v>kp-1608cgck</v>
-      </c>
-      <c r="E11" s="9" t="n">
+      <c r="C11" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0" t="n">
+        <v>8610015</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>2290328</v>
       </c>
       <c r="AMD11" s="0"/>
@@ -729,21 +886,25 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>25</v>
+    <row r="12" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kpt-1608yc")</f>
-        <v>kpt-1608yc</v>
-      </c>
-      <c r="E12" s="9" t="n">
+      <c r="C12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0" t="n">
+        <v>8610163</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>2099227</v>
       </c>
       <c r="AMD12" s="0"/>
@@ -754,21 +915,25 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>27</v>
+    <row r="13" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"kp-1608qbc-d")</f>
-        <v>kp-1608qbc-d</v>
-      </c>
-      <c r="E13" s="9" t="n">
+      <c r="C13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0" t="n">
+        <v>8608867</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>2217972</v>
       </c>
       <c r="AMD13" s="0"/>
@@ -779,21 +944,29 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>29</v>
+    <row r="14" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cd-hd2004")</f>
-        <v>cd-hd2004</v>
-      </c>
-      <c r="E14" s="9" t="n">
+      <c r="C14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>2676044</v>
       </c>
       <c r="AMD14" s="0"/>
@@ -804,34 +977,39 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="7" t="n">
+    <row r="15" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="8" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"minismdc260f-2")</f>
-        <v>minismdc260f-2</v>
-      </c>
-      <c r="E15" s="6" t="n">
+      <c r="C15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>7826420</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>1345935</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
       <c r="AMD15" s="0"/>
       <c r="AME15" s="0"/>
       <c r="AMF15" s="0"/>
@@ -842,248 +1020,331 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1210l035yr")</f>
-        <v>1210l035yr</v>
-      </c>
-      <c r="E16" s="0" t="n">
+      <c r="C16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>1822207</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"1206l050yr")</f>
-        <v>1206l050yr</v>
-      </c>
-      <c r="E17" s="0" t="n">
+      <c r="C17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>7874198</v>
+      </c>
+      <c r="H17" s="0" t="n">
         <v>1596993</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"mpz2012s601a")</f>
-        <v>mpz2012s601a</v>
-      </c>
-      <c r="E18" s="0" t="n">
+      <c r="C18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>1669753</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>39</v>
+      <c r="A19" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),742792031)</f>
+      <c r="C19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="0" t="n">
         <v>742792031</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>710742792031</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>6694092</v>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>1635734</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"s5b-xh-a-lf-sn")</f>
-        <v>s5b-xh-a-lf-sn</v>
-      </c>
-      <c r="E20" s="0" t="n">
+      <c r="C20" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>8201598</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>1516293</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"erj6geyj103v")</f>
-        <v>erj6geyj103v</v>
-      </c>
-      <c r="E21" s="0" t="n">
+      <c r="C21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>7326539</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>2057719</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"erj6geyj220v")</f>
-        <v>erj6geyj220v</v>
-      </c>
-      <c r="E22" s="0" t="n">
+      <c r="C22" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>7326602</v>
+      </c>
+      <c r="H22" s="0" t="n">
         <v>2057672</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"exb38v102jv")</f>
-        <v>exb38v102jv</v>
-      </c>
-      <c r="E23" s="0" t="n">
+      <c r="C23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>6652922</v>
+      </c>
+      <c r="H23" s="0" t="n">
         <v>2060100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"cg0603mlc-05e")</f>
-        <v>cg0603mlc-05e</v>
-      </c>
-      <c r="E24" s="0" t="n">
+      <c r="C24" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1814489</v>
+      </c>
+      <c r="H24" s="0" t="n">
         <v>1838966</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"atmega32u4-au")</f>
-        <v>atmega32u4-au</v>
-      </c>
-      <c r="E25" s="0" t="n">
+      <c r="C25" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>1310289</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>1748525</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"uln2003adr2g")</f>
-        <v>uln2003adr2g</v>
-      </c>
-      <c r="E26" s="0" t="n">
+      <c r="C26" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>2628016</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="2" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"abm8-16-000mhz-b2-t")</f>
-        <v>abm8-16-000mhz-b2-t</v>
-      </c>
-      <c r="E27" s="0" t="n">
+      <c r="C27" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>1712253</v>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>1611819</v>
       </c>
     </row>
-    <row r="28" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="7" t="n">
+    <row r="28" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="8" t="str">
-        <f aca="false">IFERROR(__xludf.dummyfunction("""COMPUTED_VALUE"""),"2213s-50g")</f>
-        <v>2213s-50g</v>
-      </c>
-      <c r="E28" s="6" t="n">
+      <c r="C28" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0" t="n">
         <v>2847228</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
       <c r="AMD28" s="0"/>
       <c r="AME28" s="0"/>
       <c r="AMF28" s="0"/>
@@ -1095,10 +1356,10 @@
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="0"/>
-      <c r="F30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="12" t="n">
+      <c r="I30" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="10" t="n">
         <f aca="false">SUM(B2:B28)</f>
         <v>48</v>
       </c>
@@ -2070,34 +2331,6 @@
     <row r="995" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="996" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://uk.farnell.com/amphenol-icc-fci/87520-0010blf/usb-2-0-type-a-plug-cable/dp/2112381?MER=sy-me-pd-mi-alte"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://uk.farnell.com/hirose-hrs/zx62d-b-5p8-30/micro-usb-2-0-type-b-rcpt-smt/dp/2554980"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://uk.farnell.com/kemet/c0805y104k4racauto/cap-0-1-f-16v-10-x7r-0805/dp/2673142?st=100nf%2016V%200805"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://uk.farnell.com/wurth-elektronik/885012007030/cap-mlcc-np0-22pf-25v-0805/dp/2533861?st=22pF%20capacitor"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://uk.farnell.com/panasonic-electronic-components/eee1ca100sr/cap-alu-elec-10uf-16v-smd/dp/9696920"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://uk.farnell.com/avx/08053c105jat2a/cap-mlcc-x7r-1uf-25v-0805/dp/2332736?st=SMD%20Multilayer%20Ceramic%20Capacitor,%200805%20[2012%20Metric],%201%20µF,%2025%20V,"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://uk.farnell.com/panasonic-electronic-components/db2w31900l/diode-schottky-30v-mini2-f3-b/dp/2284956?st=Schottky%20Rectifier,%2040%20V,%203%20A,%20Single,%20SOD-123F,%202%20Pins"/>
-    <hyperlink ref="C9" r:id="rId8" display="http://uk.farnell.com/bourns/cd1206-s01575/diode-switching-100v-150ma-1206/dp/2211947?st=CD1206-S01575"/>
-    <hyperlink ref="C10" r:id="rId9" display="http://uk.farnell.com/kingbright/kp-1608ec/led-red-8mcd-625nm-smd/dp/2463988?st=LOW%20POWER%20LED"/>
-    <hyperlink ref="C11" r:id="rId10" display="http://uk.farnell.com/kingbright/kp-1608cgck/led-0603-50mcd-green/dp/2290328?st=LOW%20POWER%20LED"/>
-    <hyperlink ref="C12" r:id="rId11" display="http://uk.farnell.com/kingbright/kpt-1608yc/led-0603-yellow-8mcd-588nm/dp/2099227?ost=2099227&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch"/>
-    <hyperlink ref="C13" r:id="rId12" display="http://uk.farnell.com/kingbright/kp-1608qbc-d/led-smd-0603-blue/dp/2217972?st=KPT-1608YC%20-%20%20LED,%20Low%20Power,%20Blue"/>
-    <hyperlink ref="C14" r:id="rId13" display="https://uk.farnell.com/bourns/cd-hd2004/diode-bridge-rect-1-ph-40v-smd/dp/2676044?krypto=HaflPpNLuHOFLHN6OxuHJMFd%2BijEvhI0duXna044V4ieLdAyHfbvP5zEqBpvqb3tSU5DiOtHH9J8%2Bn4HqqDhFw%3D%3D&amp;ddkey=https%3Aen-GB%2FElement14_United_Kingdom%2Fsearch"/>
-    <hyperlink ref="C15" r:id="rId14" display="https://uk.farnell.com/littelfuse/minismdc260f-2/polyswitch-smd-1812-2-6a/dp/1345935"/>
-    <hyperlink ref="C16" r:id="rId15" display="http://uk.farnell.com/littelfuse/1210l035yr/polyfuse-ptc-1210-0-35a/dp/1822207"/>
-    <hyperlink ref="C17" r:id="rId16" display="http://uk.farnell.com/littelfuse/1206l050yr/fuse-resettable-1206-6v-500ma/dp/1596993?ost=1596993&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch"/>
-    <hyperlink ref="C19" r:id="rId17" display="https://uk.farnell.com/wurth-elektronik/742792031/ferrite-bead-0-05ohm-3a-0805/dp/1635734?st=Ferrite%20Bead,%200805%20[2012%20Metric],%20600%20ohm,%203%20A,"/>
-    <hyperlink ref="C20" r:id="rId18" display="http://uk.farnell.com/jst-japan-solderless-terminals/s5b-xh-a-lf-sn/header-right-angle-5way/dp/1516293?ost=1516293&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch"/>
-    <hyperlink ref="C21" r:id="rId19" display="https://uk.farnell.com/panasonic-electronic-components/erj6geyj103v/res-thick-film-10k-5-0-125w-0805/dp/2057719?MER=sy-me-pd-mi-alte&amp;st=10k%20SMD%20RESISTOR"/>
-    <hyperlink ref="C22" r:id="rId20" display="https://uk.farnell.com/panasonic-electronic-components/erj6geyj220v/res-thick-film-22r-5-0-125w-0805/dp/2057672?st=SMD%20Chip%20Resistor,%2022%20ohm,%20150%20V,%20Thick%20Film,%200805%20[2012%20Metric],%20125%20mW"/>
-    <hyperlink ref="C23" r:id="rId21" display="http://uk.farnell.com/panasonic-electronic-components/exb38v102jv/resistor-cvex-array-0603x4-1k/dp/2060100?ost=2060100&amp;scope=partnumberlookahead&amp;exaMfpn=true&amp;searchref=searchlookahead&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fw%2Fsearch"/>
-    <hyperlink ref="C24" r:id="rId22" display="http://uk.farnell.com/bourns/cg0603mlc-05e/varistor-supp-esd-protect-20v/dp/1838966?ost=1838966&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch"/>
-    <hyperlink ref="C25" r:id="rId23" display="http://uk.farnell.com/microchip/atmega32u4-au/mcu-8bit-megaavr-16mhz-tqfp-44/dp/1748525?st=ATMEGA32U4"/>
-    <hyperlink ref="C26" r:id="rId24" display="http://uk.farnell.com/on-semiconductor/uln2003adr2g/trans-npn-50v-0-5a-soic-16/dp/2628016?st=ULN2003"/>
-    <hyperlink ref="C27" r:id="rId25" display="http://uk.farnell.com/abracon/abm8-16-000mhz-b2-t/crystal-16mhz-18pf-cl-3-2x2-5mm/dp/1611819?ost=1611819&amp;ddkey=http%3Aen-GB%2FElement14_United_Kingdom%2Fsearch"/>
-    <hyperlink ref="C28" r:id="rId26" display="https://uk.farnell.com/multicomp/2213s-50g/connector-header-50pos-2-54mm/dp/2847228?st=2%20row%20header%20male"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>